<commit_message>
[fix] id into excel
</commit_message>
<xml_diff>
--- a/import_radio.xlsx
+++ b/import_radio.xlsx
@@ -547,11 +547,11 @@
   </sheetPr>
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K66" activeCellId="0" sqref="K66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.83"/>
@@ -597,7 +597,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1596</v>
+        <v>1600</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>1598</v>
+        <v>1602</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>18</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>1599</v>
+        <v>1603</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -725,7 +725,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>1600</v>
+        <v>1604</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>1601</v>
+        <v>1605</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>1602</v>
+        <v>1606</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>27</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>1603</v>
+        <v>1607</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>29</v>
@@ -853,7 +853,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>1604</v>
+        <v>1608</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>30</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>1605</v>
+        <v>1609</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>31</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>1606</v>
+        <v>1610</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>33</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>1607</v>
+        <v>1611</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>35</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>1608</v>
+        <v>1612</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>37</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>1608</v>
+        <v>1613</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>37</v>
@@ -1045,7 +1045,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>1610</v>
+        <v>1614</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>40</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>1611</v>
+        <v>1615</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>42</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>1612</v>
+        <v>1616</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>44</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>1613</v>
+        <v>1617</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>46</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>1614</v>
+        <v>1618</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>47</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>1615</v>
+        <v>1619</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>49</v>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>1616</v>
+        <v>1620</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>50</v>
@@ -1269,7 +1269,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>1617</v>
+        <v>1621</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>51</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>1618</v>
+        <v>1622</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>53</v>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>1619</v>
+        <v>1623</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>54</v>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>1620</v>
+        <v>1624</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>55</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>1621</v>
+        <v>1625</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>57</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>1622</v>
+        <v>1626</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>58</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>1623</v>
+        <v>1627</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>59</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>1624</v>
+        <v>1628</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>60</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>1624</v>
+        <v>1629</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>60</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>1624</v>
+        <v>1630</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>60</v>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>1627</v>
+        <v>1631</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>64</v>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>1628</v>
+        <v>1632</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>66</v>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>1629</v>
+        <v>1633</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>68</v>
@@ -1685,7 +1685,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>1630</v>
+        <v>1634</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>70</v>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>1631</v>
+        <v>1635</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>71</v>
@@ -1749,7 +1749,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>1632</v>
+        <v>1636</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>72</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>1633</v>
+        <v>1637</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>73</v>
@@ -1813,7 +1813,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>1634</v>
+        <v>1638</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>75</v>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>1635</v>
+        <v>1639</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>76</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>1636</v>
+        <v>1640</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>78</v>
@@ -1909,7 +1909,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>1637</v>
+        <v>1641</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>80</v>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>1638</v>
+        <v>1642</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>82</v>
@@ -1973,7 +1973,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>1639</v>
+        <v>1643</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>84</v>
@@ -2005,7 +2005,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>1639</v>
+        <v>1644</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>84</v>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>1641</v>
+        <v>1645</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>87</v>
@@ -2069,7 +2069,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>1642</v>
+        <v>1646</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>89</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>1643</v>
+        <v>1647</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>90</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>1644</v>
+        <v>1648</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>91</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>1645</v>
+        <v>1649</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>93</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>1646</v>
+        <v>1650</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>96</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>1647</v>
+        <v>1651</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>98</v>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>1648</v>
+        <v>1652</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>102</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>1649</v>
+        <v>1653</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>104</v>
@@ -2321,7 +2321,7 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>1650</v>
+        <v>1654</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>106</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>1651</v>
+        <v>1655</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>107</v>
@@ -2383,7 +2383,7 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>1652</v>
+        <v>1656</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>109</v>
@@ -2415,7 +2415,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>1652</v>
+        <v>1657</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>109</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>1652</v>
+        <v>1658</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>109</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>1652</v>
+        <v>1659</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>109</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>1656</v>
+        <v>1660</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>112</v>
@@ -2543,7 +2543,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>1657</v>
+        <v>1661</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>114</v>
@@ -2575,7 +2575,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>1658</v>
+        <v>1662</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>116</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>1659</v>
+        <v>1663</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>118</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>1659</v>
+        <v>1664</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>118</v>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>1659</v>
+        <v>1665</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>118</v>
@@ -2703,7 +2703,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>1662</v>
+        <v>1666</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>122</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>1662</v>
+        <v>1667</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>122</v>
@@ -2767,7 +2767,7 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>1664</v>
+        <v>1668</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>125</v>
@@ -2799,7 +2799,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>1665</v>
+        <v>1669</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>127</v>
@@ -2831,7 +2831,7 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>1666</v>
+        <v>1670</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>128</v>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>1666</v>
+        <v>1671</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>128</v>
@@ -2895,7 +2895,7 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>1668</v>
+        <v>1672</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>131</v>
@@ -2927,7 +2927,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <v>1669</v>
+        <v>1673</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>133</v>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
-        <v>1669</v>
+        <v>1674</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>133</v>

</xml_diff>